<commit_message>
Compelted weekly task, set up Payment class. Updated Gant Chart to reflect progress.
</commit_message>
<xml_diff>
--- a/CS401ProjectGnattChartV2Fastrak.xlsx
+++ b/CS401ProjectGnattChartV2Fastrak.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C8C4A6A7-E1AC-429D-B960-94BCE1D8EB58}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3016D7EC-D1BC-5146-8ECF-D44A246002E9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ProjectSchedule" sheetId="11" r:id="rId1"/>
@@ -259,13 +259,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <numFmts count="6">
+  <numFmts count="5">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="m/d/yy;@"/>
     <numFmt numFmtId="165" formatCode="ddd\,\ m/d/yyyy"/>
     <numFmt numFmtId="166" formatCode="mmm\ d\,\ yyyy"/>
     <numFmt numFmtId="167" formatCode="d"/>
-    <numFmt numFmtId="168" formatCode="m/d/yy"/>
   </numFmts>
   <fonts count="23" x14ac:knownFonts="1">
     <font>
@@ -766,7 +765,7 @@
     <xf numFmtId="9" fontId="22" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="22" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="22" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -778,7 +777,7 @@
     <xf numFmtId="9" fontId="22" fillId="6" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="22" fillId="6" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="22" fillId="6" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -790,7 +789,7 @@
     <xf numFmtId="9" fontId="22" fillId="7" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="22" fillId="7" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="22" fillId="7" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -802,7 +801,7 @@
     <xf numFmtId="9" fontId="22" fillId="8" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="22" fillId="8" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="22" fillId="8" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -814,7 +813,7 @@
     <xf numFmtId="9" fontId="22" fillId="9" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="22" fillId="9" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="22" fillId="9" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -826,7 +825,7 @@
     <xf numFmtId="9" fontId="22" fillId="10" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="22" fillId="10" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="22" fillId="10" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -838,7 +837,7 @@
     <xf numFmtId="9" fontId="22" fillId="11" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="22" fillId="11" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="22" fillId="11" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="12" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -850,7 +849,7 @@
     <xf numFmtId="9" fontId="22" fillId="12" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="22" fillId="12" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="22" fillId="12" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="22" fillId="6" borderId="11" xfId="12" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1623,25 +1622,25 @@
   </sheetPr>
   <dimension ref="A1:BS29"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScale="64" zoomScaleNormal="64" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K11" sqref="K11"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScale="83" zoomScaleNormal="64" zoomScalePageLayoutView="70" workbookViewId="0">
+      <pane ySplit="6" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="2.7265625" style="28" customWidth="1"/>
-    <col min="2" max="2" width="19.81640625" customWidth="1"/>
-    <col min="3" max="3" width="35.7265625" customWidth="1"/>
-    <col min="4" max="4" width="10.7265625" customWidth="1"/>
-    <col min="5" max="5" width="10.453125" style="5" customWidth="1"/>
-    <col min="6" max="6" width="10.453125" customWidth="1"/>
-    <col min="7" max="7" width="2.7265625" customWidth="1"/>
-    <col min="8" max="8" width="6.1796875" hidden="1" customWidth="1"/>
-    <col min="9" max="71" width="2.54296875" customWidth="1"/>
+    <col min="1" max="1" width="2.6640625" style="28" customWidth="1"/>
+    <col min="2" max="2" width="19.83203125" customWidth="1"/>
+    <col min="3" max="3" width="35.6640625" customWidth="1"/>
+    <col min="4" max="4" width="10.6640625" customWidth="1"/>
+    <col min="5" max="5" width="10.5" style="5" customWidth="1"/>
+    <col min="6" max="6" width="10.5" customWidth="1"/>
+    <col min="7" max="7" width="2.6640625" customWidth="1"/>
+    <col min="8" max="8" width="6.1640625" hidden="1" customWidth="1"/>
+    <col min="9" max="71" width="2.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:71" ht="30" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="1" spans="1:71" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="29" t="s">
         <v>24</v>
       </c>
@@ -1657,7 +1656,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:71" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:71" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="28" t="s">
         <v>22</v>
       </c>
@@ -1668,7 +1667,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:71" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:71" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="28" t="s">
         <v>25</v>
       </c>
@@ -1682,7 +1681,7 @@
       </c>
       <c r="F3" s="71"/>
     </row>
-    <row r="4" spans="1:71" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:71" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="29" t="s">
         <v>26</v>
       </c>
@@ -1784,7 +1783,7 @@
       <c r="BR4" s="69"/>
       <c r="BS4" s="70"/>
     </row>
-    <row r="5" spans="1:71" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:71" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="29" t="s">
         <v>27</v>
       </c>
@@ -2047,7 +2046,7 @@
         <v>43947</v>
       </c>
     </row>
-    <row r="6" spans="1:71" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:71" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="29" t="s">
         <v>28</v>
       </c>
@@ -2321,7 +2320,7 @@
         <v>S</v>
       </c>
     </row>
-    <row r="7" spans="1:71" ht="30" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:71" ht="30" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="28" t="s">
         <v>23</v>
       </c>
@@ -2395,7 +2394,7 @@
       <c r="BR7" s="15"/>
       <c r="BS7" s="15"/>
     </row>
-    <row r="8" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="29" t="s">
         <v>29</v>
       </c>
@@ -2475,7 +2474,7 @@
       <c r="BR8" s="15"/>
       <c r="BS8" s="15"/>
     </row>
-    <row r="9" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="29" t="s">
         <v>30</v>
       </c>
@@ -2561,7 +2560,7 @@
       <c r="BR9" s="15"/>
       <c r="BS9" s="15"/>
     </row>
-    <row r="10" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="29" t="s">
         <v>31</v>
       </c>
@@ -2570,7 +2569,7 @@
       </c>
       <c r="C10" s="40"/>
       <c r="D10" s="67">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="E10" s="42">
         <v>43902</v>
@@ -2647,7 +2646,7 @@
       <c r="BR10" s="15"/>
       <c r="BS10" s="15"/>
     </row>
-    <row r="11" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="29" t="s">
         <v>32</v>
       </c>
@@ -2727,7 +2726,7 @@
       <c r="BR11" s="15"/>
       <c r="BS11" s="15"/>
     </row>
-    <row r="12" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="28"/>
       <c r="B12" s="47" t="s">
         <v>47</v>
@@ -2808,7 +2807,7 @@
       <c r="BR12" s="15"/>
       <c r="BS12" s="15"/>
     </row>
-    <row r="13" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="28"/>
       <c r="B13" s="47" t="s">
         <v>34</v>
@@ -2889,14 +2888,14 @@
       <c r="BR13" s="15"/>
       <c r="BS13" s="15"/>
     </row>
-    <row r="14" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="28"/>
       <c r="B14" s="47" t="s">
         <v>46</v>
       </c>
       <c r="C14" s="48"/>
       <c r="D14" s="49">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E14" s="50">
         <v>43913</v>
@@ -2973,7 +2972,7 @@
       <c r="BR14" s="15"/>
       <c r="BS14" s="15"/>
     </row>
-    <row r="15" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="28" t="s">
         <v>36</v>
       </c>
@@ -3053,7 +3052,7 @@
       <c r="BR15" s="15"/>
       <c r="BS15" s="15"/>
     </row>
-    <row r="16" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="28"/>
       <c r="B16" s="55" t="s">
         <v>42</v>
@@ -3137,7 +3136,7 @@
       <c r="BR16" s="15"/>
       <c r="BS16" s="15"/>
     </row>
-    <row r="17" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="28"/>
       <c r="B17" s="55" t="s">
         <v>48</v>
@@ -3221,7 +3220,7 @@
       <c r="BR17" s="15"/>
       <c r="BS17" s="15"/>
     </row>
-    <row r="18" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="28"/>
       <c r="B18" s="55" t="s">
         <v>49</v>
@@ -3305,7 +3304,7 @@
       <c r="BR18" s="15"/>
       <c r="BS18" s="15"/>
     </row>
-    <row r="19" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="28" t="s">
         <v>38</v>
       </c>
@@ -3385,7 +3384,7 @@
       <c r="BR19" s="15"/>
       <c r="BS19" s="15"/>
     </row>
-    <row r="20" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="28"/>
       <c r="B20" s="63" t="s">
         <v>50</v>
@@ -3469,7 +3468,7 @@
       <c r="BR20" s="15"/>
       <c r="BS20" s="15"/>
     </row>
-    <row r="21" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="28"/>
       <c r="B21" s="63" t="s">
         <v>53</v>
@@ -3553,7 +3552,7 @@
       <c r="BR21" s="15"/>
       <c r="BS21" s="15"/>
     </row>
-    <row r="22" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="28"/>
       <c r="B22" s="63" t="s">
         <v>51</v>
@@ -3637,7 +3636,7 @@
       <c r="BR22" s="15"/>
       <c r="BS22" s="15"/>
     </row>
-    <row r="23" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="28"/>
       <c r="B23" s="63" t="s">
         <v>52</v>
@@ -3721,7 +3720,7 @@
       <c r="BR23" s="15"/>
       <c r="BS23" s="15"/>
     </row>
-    <row r="24" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="28" t="s">
         <v>38</v>
       </c>
@@ -3801,7 +3800,7 @@
       <c r="BR24" s="15"/>
       <c r="BS24" s="15"/>
     </row>
-    <row r="25" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="28"/>
       <c r="B25" s="63" t="s">
         <v>54</v>
@@ -3885,7 +3884,7 @@
       <c r="BR25" s="15"/>
       <c r="BS25" s="15"/>
     </row>
-    <row r="26" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="28"/>
       <c r="B26" s="63" t="s">
         <v>55</v>
@@ -3969,7 +3968,7 @@
       <c r="BR26" s="15"/>
       <c r="BS26" s="15"/>
     </row>
-    <row r="27" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="28" t="s">
         <v>38</v>
       </c>
@@ -4049,7 +4048,7 @@
       <c r="BR27" s="15"/>
       <c r="BS27" s="15"/>
     </row>
-    <row r="28" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="28"/>
       <c r="B28" s="63" t="s">
         <v>56</v>
@@ -4133,7 +4132,7 @@
       <c r="BR28" s="15"/>
       <c r="BS28" s="15"/>
     </row>
-    <row r="29" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="28"/>
       <c r="B29" s="63" t="s">
         <v>57</v>
@@ -4384,86 +4383,86 @@
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="87.1796875" style="18" customWidth="1"/>
-    <col min="2" max="16384" width="9.1796875" style="2"/>
+    <col min="1" max="1" width="87.1640625" style="18" customWidth="1"/>
+    <col min="2" max="16384" width="9.1640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="46.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:2" s="20" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" ht="46.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="2" spans="1:2" s="20" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
         <v>10</v>
       </c>
       <c r="B2" s="19"/>
     </row>
-    <row r="3" spans="1:2" s="24" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" s="24" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="25" t="s">
         <v>15</v>
       </c>
       <c r="B3" s="25"/>
     </row>
-    <row r="4" spans="1:2" s="21" customFormat="1" ht="26" x14ac:dyDescent="0.6">
+    <row r="4" spans="1:2" s="21" customFormat="1" ht="26" x14ac:dyDescent="0.3">
       <c r="A4" s="22" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="74.150000000000006" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" ht="74.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="23" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="22" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:2" s="18" customFormat="1" ht="205" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" s="18" customFormat="1" ht="205" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="27" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:2" s="21" customFormat="1" ht="26" x14ac:dyDescent="0.6">
+    <row r="8" spans="1:2" s="21" customFormat="1" ht="26" x14ac:dyDescent="0.3">
       <c r="A8" s="22" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="58" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" ht="48" x14ac:dyDescent="0.2">
       <c r="A9" s="23" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:2" s="18" customFormat="1" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" s="18" customFormat="1" ht="28" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="26" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:2" s="21" customFormat="1" ht="26" x14ac:dyDescent="0.6">
+    <row r="11" spans="1:2" s="21" customFormat="1" ht="26" x14ac:dyDescent="0.3">
       <c r="A11" s="22" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="29" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" ht="32" x14ac:dyDescent="0.2">
       <c r="A12" s="23" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:2" s="18" customFormat="1" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" s="18" customFormat="1" ht="28" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="26" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:2" s="21" customFormat="1" ht="26" x14ac:dyDescent="0.6">
+    <row r="14" spans="1:2" s="21" customFormat="1" ht="26" x14ac:dyDescent="0.3">
       <c r="A14" s="22" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" ht="75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="23" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="72.5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" ht="64" x14ac:dyDescent="0.2">
       <c r="A16" s="23" t="s">
         <v>14</v>
       </c>

</xml_diff>

<commit_message>
version 1.2 of gnatt chart
</commit_message>
<xml_diff>
--- a/CS401ProjectGnattChartV2Fastrak.xlsx
+++ b/CS401ProjectGnattChartV2Fastrak.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C8C4A6A7-E1AC-429D-B960-94BCE1D8EB58}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="8_{C8C4A6A7-E1AC-429D-B960-94BCE1D8EB58}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{BA17301B-98B6-4214-8E14-ECDAAAAC90A6}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -856,6 +856,13 @@
     <xf numFmtId="9" fontId="22" fillId="6" borderId="11" xfId="12" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="7">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="7" applyBorder="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="166" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -868,13 +875,6 @@
     <xf numFmtId="165" fontId="7" fillId="0" borderId="3" xfId="8" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="7">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="7" applyBorder="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="13">
     <cellStyle name="Comma" xfId="3" builtinId="3" customBuiltin="1"/>
@@ -1625,7 +1625,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScale="64" zoomScaleNormal="64" zoomScalePageLayoutView="70" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K11" sqref="K11"/>
+      <selection pane="bottomLeft" activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1673,127 +1673,127 @@
         <v>25</v>
       </c>
       <c r="B3" s="34"/>
-      <c r="C3" s="72" t="s">
+      <c r="C3" s="68" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="73"/>
-      <c r="E3" s="71">
+      <c r="D3" s="69"/>
+      <c r="E3" s="74">
         <v>43878</v>
       </c>
-      <c r="F3" s="71"/>
+      <c r="F3" s="74"/>
     </row>
     <row r="4" spans="1:71" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="C4" s="72" t="s">
+      <c r="C4" s="68" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="73"/>
+      <c r="D4" s="69"/>
       <c r="E4" s="6">
         <v>2</v>
       </c>
-      <c r="I4" s="68">
+      <c r="I4" s="71">
         <f>I5</f>
         <v>43885</v>
       </c>
-      <c r="J4" s="69"/>
-      <c r="K4" s="69"/>
-      <c r="L4" s="69"/>
-      <c r="M4" s="69"/>
-      <c r="N4" s="69"/>
-      <c r="O4" s="70"/>
-      <c r="P4" s="68">
+      <c r="J4" s="72"/>
+      <c r="K4" s="72"/>
+      <c r="L4" s="72"/>
+      <c r="M4" s="72"/>
+      <c r="N4" s="72"/>
+      <c r="O4" s="73"/>
+      <c r="P4" s="71">
         <f>P5</f>
         <v>43892</v>
       </c>
-      <c r="Q4" s="69"/>
-      <c r="R4" s="69"/>
-      <c r="S4" s="69"/>
-      <c r="T4" s="69"/>
-      <c r="U4" s="69"/>
-      <c r="V4" s="70"/>
-      <c r="W4" s="68">
+      <c r="Q4" s="72"/>
+      <c r="R4" s="72"/>
+      <c r="S4" s="72"/>
+      <c r="T4" s="72"/>
+      <c r="U4" s="72"/>
+      <c r="V4" s="73"/>
+      <c r="W4" s="71">
         <f>W5</f>
         <v>43899</v>
       </c>
-      <c r="X4" s="69"/>
-      <c r="Y4" s="69"/>
-      <c r="Z4" s="69"/>
-      <c r="AA4" s="69"/>
-      <c r="AB4" s="69"/>
-      <c r="AC4" s="70"/>
-      <c r="AD4" s="68">
+      <c r="X4" s="72"/>
+      <c r="Y4" s="72"/>
+      <c r="Z4" s="72"/>
+      <c r="AA4" s="72"/>
+      <c r="AB4" s="72"/>
+      <c r="AC4" s="73"/>
+      <c r="AD4" s="71">
         <f>AD5</f>
         <v>43906</v>
       </c>
-      <c r="AE4" s="69"/>
-      <c r="AF4" s="69"/>
-      <c r="AG4" s="69"/>
-      <c r="AH4" s="69"/>
-      <c r="AI4" s="69"/>
-      <c r="AJ4" s="70"/>
-      <c r="AK4" s="68">
+      <c r="AE4" s="72"/>
+      <c r="AF4" s="72"/>
+      <c r="AG4" s="72"/>
+      <c r="AH4" s="72"/>
+      <c r="AI4" s="72"/>
+      <c r="AJ4" s="73"/>
+      <c r="AK4" s="71">
         <f>AK5</f>
         <v>43913</v>
       </c>
-      <c r="AL4" s="69"/>
-      <c r="AM4" s="69"/>
-      <c r="AN4" s="69"/>
-      <c r="AO4" s="69"/>
-      <c r="AP4" s="69"/>
-      <c r="AQ4" s="70"/>
-      <c r="AR4" s="68">
+      <c r="AL4" s="72"/>
+      <c r="AM4" s="72"/>
+      <c r="AN4" s="72"/>
+      <c r="AO4" s="72"/>
+      <c r="AP4" s="72"/>
+      <c r="AQ4" s="73"/>
+      <c r="AR4" s="71">
         <f>AR5</f>
         <v>43920</v>
       </c>
-      <c r="AS4" s="69"/>
-      <c r="AT4" s="69"/>
-      <c r="AU4" s="69"/>
-      <c r="AV4" s="69"/>
-      <c r="AW4" s="69"/>
-      <c r="AX4" s="70"/>
-      <c r="AY4" s="68">
+      <c r="AS4" s="72"/>
+      <c r="AT4" s="72"/>
+      <c r="AU4" s="72"/>
+      <c r="AV4" s="72"/>
+      <c r="AW4" s="72"/>
+      <c r="AX4" s="73"/>
+      <c r="AY4" s="71">
         <f>AY5</f>
         <v>43927</v>
       </c>
-      <c r="AZ4" s="69"/>
-      <c r="BA4" s="69"/>
-      <c r="BB4" s="69"/>
-      <c r="BC4" s="69"/>
-      <c r="BD4" s="69"/>
-      <c r="BE4" s="70"/>
-      <c r="BF4" s="68">
+      <c r="AZ4" s="72"/>
+      <c r="BA4" s="72"/>
+      <c r="BB4" s="72"/>
+      <c r="BC4" s="72"/>
+      <c r="BD4" s="72"/>
+      <c r="BE4" s="73"/>
+      <c r="BF4" s="71">
         <f>BF5</f>
         <v>43934</v>
       </c>
-      <c r="BG4" s="69"/>
-      <c r="BH4" s="69"/>
-      <c r="BI4" s="69"/>
-      <c r="BJ4" s="69"/>
-      <c r="BK4" s="69"/>
-      <c r="BL4" s="70"/>
-      <c r="BM4" s="68">
+      <c r="BG4" s="72"/>
+      <c r="BH4" s="72"/>
+      <c r="BI4" s="72"/>
+      <c r="BJ4" s="72"/>
+      <c r="BK4" s="72"/>
+      <c r="BL4" s="73"/>
+      <c r="BM4" s="71">
         <f>BM5</f>
         <v>43941</v>
       </c>
-      <c r="BN4" s="69"/>
-      <c r="BO4" s="69"/>
-      <c r="BP4" s="69"/>
-      <c r="BQ4" s="69"/>
-      <c r="BR4" s="69"/>
-      <c r="BS4" s="70"/>
+      <c r="BN4" s="72"/>
+      <c r="BO4" s="72"/>
+      <c r="BP4" s="72"/>
+      <c r="BQ4" s="72"/>
+      <c r="BR4" s="72"/>
+      <c r="BS4" s="73"/>
     </row>
     <row r="5" spans="1:71" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="B5" s="74"/>
-      <c r="C5" s="74"/>
-      <c r="D5" s="74"/>
-      <c r="E5" s="74"/>
-      <c r="F5" s="74"/>
-      <c r="G5" s="74"/>
+      <c r="B5" s="70"/>
+      <c r="C5" s="70"/>
+      <c r="D5" s="70"/>
+      <c r="E5" s="70"/>
+      <c r="F5" s="70"/>
+      <c r="G5" s="70"/>
       <c r="I5" s="10">
         <f>Project_Start-WEEKDAY(Project_Start,1)+2+7*(Display_Week-1)</f>
         <v>43885</v>
@@ -2570,7 +2570,7 @@
       </c>
       <c r="C10" s="40"/>
       <c r="D10" s="67">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="E10" s="42">
         <v>43902</v>
@@ -2815,7 +2815,7 @@
       </c>
       <c r="C13" s="48"/>
       <c r="D13" s="49">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E13" s="50">
         <v>43913</v>
@@ -2896,7 +2896,7 @@
       </c>
       <c r="C14" s="48"/>
       <c r="D14" s="49">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E14" s="50">
         <v>43913</v>
@@ -4219,11 +4219,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="AK4:AQ4"/>
-    <mergeCell ref="AR4:AX4"/>
     <mergeCell ref="BM4:BS4"/>
     <mergeCell ref="AY4:BE4"/>
     <mergeCell ref="BF4:BL4"/>
@@ -4232,6 +4227,11 @@
     <mergeCell ref="P4:V4"/>
     <mergeCell ref="W4:AC4"/>
     <mergeCell ref="AD4:AJ4"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="AK4:AQ4"/>
+    <mergeCell ref="AR4:AX4"/>
   </mergeCells>
   <phoneticPr fontId="20" type="noConversion"/>
   <conditionalFormatting sqref="D7">

</xml_diff>

<commit_message>
new version1.2 of gnatt chart
</commit_message>
<xml_diff>
--- a/CS401ProjectGnattChartV2Fastrak.xlsx
+++ b/CS401ProjectGnattChartV2Fastrak.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="3" documentId="8_{C8C4A6A7-E1AC-429D-B960-94BCE1D8EB58}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{BA17301B-98B6-4214-8E14-ECDAAAAC90A6}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57113943-CFED-4402-A36B-C350B1AE25EA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -259,13 +259,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <numFmts count="6">
+  <numFmts count="5">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="m/d/yy;@"/>
     <numFmt numFmtId="165" formatCode="ddd\,\ m/d/yyyy"/>
     <numFmt numFmtId="166" formatCode="mmm\ d\,\ yyyy"/>
     <numFmt numFmtId="167" formatCode="d"/>
-    <numFmt numFmtId="168" formatCode="m/d/yy"/>
   </numFmts>
   <fonts count="23" x14ac:knownFonts="1">
     <font>
@@ -766,7 +765,7 @@
     <xf numFmtId="9" fontId="22" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="22" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="22" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -778,7 +777,7 @@
     <xf numFmtId="9" fontId="22" fillId="6" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="22" fillId="6" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="22" fillId="6" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -790,7 +789,7 @@
     <xf numFmtId="9" fontId="22" fillId="7" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="22" fillId="7" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="22" fillId="7" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -802,7 +801,7 @@
     <xf numFmtId="9" fontId="22" fillId="8" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="22" fillId="8" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="22" fillId="8" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -814,7 +813,7 @@
     <xf numFmtId="9" fontId="22" fillId="9" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="22" fillId="9" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="22" fillId="9" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -826,7 +825,7 @@
     <xf numFmtId="9" fontId="22" fillId="10" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="22" fillId="10" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="22" fillId="10" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -838,7 +837,7 @@
     <xf numFmtId="9" fontId="22" fillId="11" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="22" fillId="11" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="22" fillId="11" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="12" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -850,7 +849,7 @@
     <xf numFmtId="9" fontId="22" fillId="12" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="22" fillId="12" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="22" fillId="12" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="22" fillId="6" borderId="11" xfId="12" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1623,22 +1622,22 @@
   </sheetPr>
   <dimension ref="A1:BS29"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScale="64" zoomScaleNormal="64" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScale="83" zoomScaleNormal="64" zoomScalePageLayoutView="70" workbookViewId="0">
+      <pane ySplit="6" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="2.7265625" style="28" customWidth="1"/>
+    <col min="1" max="1" width="2.6328125" style="28" customWidth="1"/>
     <col min="2" max="2" width="19.81640625" customWidth="1"/>
-    <col min="3" max="3" width="35.7265625" customWidth="1"/>
-    <col min="4" max="4" width="10.7265625" customWidth="1"/>
+    <col min="3" max="3" width="35.6328125" customWidth="1"/>
+    <col min="4" max="4" width="10.6328125" customWidth="1"/>
     <col min="5" max="5" width="10.453125" style="5" customWidth="1"/>
     <col min="6" max="6" width="10.453125" customWidth="1"/>
-    <col min="7" max="7" width="2.7265625" customWidth="1"/>
+    <col min="7" max="7" width="2.6328125" customWidth="1"/>
     <col min="8" max="8" width="6.1796875" hidden="1" customWidth="1"/>
-    <col min="9" max="71" width="2.54296875" customWidth="1"/>
+    <col min="9" max="71" width="2.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:71" ht="30" customHeight="1" x14ac:dyDescent="0.65">
@@ -4408,7 +4407,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="74.150000000000006" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" ht="74.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="23" t="s">
         <v>18</v>
       </c>

</xml_diff>

<commit_message>
skeleton for Client class and Testing  Plan version1.2
</commit_message>
<xml_diff>
--- a/CS401ProjectGnattChartV2Fastrak.xlsx
+++ b/CS401ProjectGnattChartV2Fastrak.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8718F3FA-681D-47AB-9EEA-E7995821AE2F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="114_{9B748DD8-A117-4469-9E25-801C939C2C02}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{7F0DC282-4CF7-438D-AF57-E1618862520B}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1624,8 +1624,8 @@
   <dimension ref="A1:BS29"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScale="64" zoomScaleNormal="64" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D12" sqref="D12"/>
+      <pane ySplit="6" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -3060,7 +3060,7 @@
       </c>
       <c r="C16" s="56"/>
       <c r="D16" s="57">
-        <v>0</v>
+        <v>0.85</v>
       </c>
       <c r="E16" s="58">
         <v>43920</v>

</xml_diff>